<commit_message>
fix: update SDMUH2_DATA_LENGKAP_UPDATE_19-05-24.xlsx with latest data
</commit_message>
<xml_diff>
--- a/SDMUH2_DATA_LENGKAP_UPDATE_19-05-24.xlsx
+++ b/SDMUH2_DATA_LENGKAP_UPDATE_19-05-24.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hai_ru/Workspace/norapos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hai_ru/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31499F65-FC54-6D47-B2FE-87BFD812B7F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14F8ABE-9440-DB4C-8D14-7311948D8F73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="20640" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17344,7 +17344,7 @@
       <patternFill patternType="none"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -17379,17 +17379,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -17400,22 +17389,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -17429,26 +17407,20 @@
     <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -17756,8 +17728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:P1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17812,61 +17784,46 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="13" t="s">
+    <row r="6" spans="2:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D6" s="12" t="s">
         <v>5752</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E6" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G6" s="12" t="s">
         <v>5746</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="K6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="L5" s="11" t="s">
+      <c r="L6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="M5" s="14" t="s">
+      <c r="M6" s="14" t="s">
         <v>5750</v>
       </c>
-      <c r="N5" s="16" t="s">
+      <c r="N6" s="15" t="s">
         <v>5751</v>
       </c>
-    </row>
-    <row r="6" spans="2:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="13"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="17"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B7" s="7">
@@ -61367,21 +61324,6 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C7:N1000">
     <sortCondition ref="G7:G1000"/>
   </sortState>
-  <mergeCells count="13">
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-  </mergeCells>
   <pageMargins left="0.69930555555555995" right="0.69930555555555995" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>

</xml_diff>